<commit_message>
correções na fase de enchimento de grãos
</commit_message>
<xml_diff>
--- a/inst/MaizeParams.xlsx
+++ b/inst/MaizeParams.xlsx
@@ -602,7 +602,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K5" sqref="K5:K8"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -688,7 +688,7 @@
         <v>170</v>
       </c>
       <c r="G2" s="3">
-        <v>1200</v>
+        <v>1600</v>
       </c>
       <c r="H2" s="3">
         <v>4</v>

</xml_diff>

<commit_message>
correções no modelo do milho e no diurnalmet.R
</commit_message>
<xml_diff>
--- a/inst/MaizeParams.xlsx
+++ b/inst/MaizeParams.xlsx
@@ -211,9 +211,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,10 +309,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -626,13 +623,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K2" sqref="K2:K8"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -722,11 +719,11 @@
       <c r="F2" s="3">
         <v>170</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>1620</v>
       </c>
-      <c r="H2" s="10">
-        <v>0.4</v>
+      <c r="H2" s="11">
+        <v>0.45</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -778,11 +775,11 @@
       <c r="F3" s="3">
         <v>170</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="3">
         <v>1600</v>
       </c>
-      <c r="H3" s="10">
-        <v>0.4</v>
+      <c r="H3" s="11">
+        <v>0.45</v>
       </c>
       <c r="I3" s="3">
         <v>4</v>
@@ -794,7 +791,7 @@
         <v>4</v>
       </c>
       <c r="L3" s="3">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M3" s="3">
         <v>1.1499999999999999</v>
@@ -834,11 +831,11 @@
       <c r="F4" s="3">
         <v>170</v>
       </c>
-      <c r="G4" s="11">
-        <v>1640</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.4</v>
+      <c r="G4" s="3">
+        <v>1650</v>
+      </c>
+      <c r="H4" s="11">
+        <v>0.51</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
@@ -850,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="3">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M4" s="3">
         <v>1.1499999999999999</v>
@@ -890,11 +887,11 @@
       <c r="F5" s="3">
         <v>170</v>
       </c>
-      <c r="G5" s="11">
-        <v>2240</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0.4</v>
+      <c r="G5" s="3">
+        <v>1780</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.52</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -906,7 +903,7 @@
         <v>4</v>
       </c>
       <c r="L5" s="3">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="M5" s="3">
         <v>1.1499999999999999</v>
@@ -946,11 +943,11 @@
       <c r="F6" s="3">
         <v>170</v>
       </c>
-      <c r="G6" s="11">
-        <v>1750</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.4</v>
+      <c r="G6" s="3">
+        <v>1500</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0.51</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
@@ -962,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="L6" s="3">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="M6" s="3">
         <v>1.1499999999999999</v>
@@ -1002,11 +999,11 @@
       <c r="F7" s="3">
         <v>170</v>
       </c>
-      <c r="G7" s="11">
-        <v>1600</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0.4</v>
+      <c r="G7" s="3">
+        <v>1680</v>
+      </c>
+      <c r="H7" s="11">
+        <v>0.5</v>
       </c>
       <c r="I7" s="3">
         <v>4</v>
@@ -1018,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="L7" s="3">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="M7" s="3">
         <v>1.1499999999999999</v>
@@ -1058,11 +1055,11 @@
       <c r="F8" s="3">
         <v>170</v>
       </c>
-      <c r="G8" s="11">
-        <v>1650</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0.4</v>
+      <c r="G8" s="3">
+        <v>1580</v>
+      </c>
+      <c r="H8" s="11">
+        <v>0.48</v>
       </c>
       <c r="I8" s="3">
         <v>4</v>
@@ -1074,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="L8" s="3">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="M8" s="3">
         <v>1.1499999999999999</v>
@@ -1094,6 +1091,21 @@
       <c r="R8" s="3">
         <v>0.26</v>
       </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
alterações no modelo do milho
</commit_message>
<xml_diff>
--- a/inst/MaizeParams.xlsx
+++ b/inst/MaizeParams.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="62">
   <si>
     <t>VARNAME</t>
   </si>
@@ -211,6 +211,33 @@
   </si>
   <si>
     <t>SLAf</t>
+  </si>
+  <si>
+    <t>Asgrow</t>
+  </si>
+  <si>
+    <t>DeKalb</t>
+  </si>
+  <si>
+    <t>Pioneer</t>
+  </si>
+  <si>
+    <t>GENERIC</t>
+  </si>
+  <si>
+    <t>SLAk</t>
+  </si>
+  <si>
+    <t>MLA</t>
+  </si>
+  <si>
+    <t>VMLA</t>
+  </si>
+  <si>
+    <t>MLAc</t>
+  </si>
+  <si>
+    <t>MALA</t>
   </si>
 </sst>
 </file>
@@ -629,13 +656,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -647,10 +674,10 @@
     <col min="5" max="5" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="8.89453125" style="3"/>
     <col min="8" max="8" width="8.83984375" style="3"/>
-    <col min="9" max="18" width="8.89453125" style="3"/>
+    <col min="9" max="16" width="8.89453125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -691,28 +718,37 @@
         <v>14</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="S1" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>61</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" t="s">
+        <v>59</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -753,33 +789,42 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="N2" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O2" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P2" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q2" s="3">
-        <v>8.6999999999999993</v>
+        <v>60</v>
       </c>
       <c r="R2" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S2" s="3">
-        <v>60</v>
+        <v>35</v>
+      </c>
+      <c r="S2">
+        <v>-0.45</v>
       </c>
       <c r="T2" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>450</v>
+      </c>
+      <c r="U2" s="3">
+        <v>850</v>
+      </c>
+      <c r="V2">
+        <v>11</v>
+      </c>
+      <c r="W2" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C3" s="3">
         <v>15</v>
@@ -809,39 +854,48 @@
         <v>4</v>
       </c>
       <c r="L3" s="3">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="M3" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N3" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O3" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P3" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q3" s="3">
-        <v>8.6999999999999993</v>
+        <v>50</v>
       </c>
       <c r="R3" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S3" s="3">
-        <v>55</v>
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>-0.45</v>
       </c>
       <c r="T3" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>450</v>
+      </c>
+      <c r="U3" s="3">
+        <v>850</v>
+      </c>
+      <c r="V3">
+        <v>11</v>
+      </c>
+      <c r="W3" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3">
         <v>15</v>
@@ -856,10 +910,10 @@
         <v>170</v>
       </c>
       <c r="G4" s="3">
-        <v>1650</v>
+        <v>1660</v>
       </c>
       <c r="H4" s="11">
-        <v>0.51</v>
+        <v>0.45</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
@@ -871,39 +925,48 @@
         <v>4</v>
       </c>
       <c r="L4" s="3">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="M4" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N4" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O4" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P4" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q4" s="3">
-        <v>8.6999999999999993</v>
+        <v>50</v>
       </c>
       <c r="R4" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S4" s="3">
-        <v>55</v>
+        <v>35</v>
+      </c>
+      <c r="S4">
+        <v>-0.45</v>
       </c>
       <c r="T4" s="3">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>620</v>
+      </c>
+      <c r="U4" s="3">
+        <v>850</v>
+      </c>
+      <c r="V4">
+        <v>11</v>
+      </c>
+      <c r="W4" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3">
         <v>15</v>
@@ -918,10 +981,10 @@
         <v>170</v>
       </c>
       <c r="G5" s="3">
-        <v>1765</v>
+        <v>1760</v>
       </c>
       <c r="H5" s="11">
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -933,39 +996,48 @@
         <v>4</v>
       </c>
       <c r="L5" s="3">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="M5" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N5" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O5" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P5" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q5" s="3">
-        <v>8.6999999999999993</v>
+        <v>50</v>
       </c>
       <c r="R5" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S5" s="3">
-        <v>53</v>
+        <v>34</v>
+      </c>
+      <c r="S5">
+        <v>-0.45</v>
       </c>
       <c r="T5" s="3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>490</v>
+      </c>
+      <c r="U5" s="3">
+        <v>850</v>
+      </c>
+      <c r="V5">
+        <v>11</v>
+      </c>
+      <c r="W5" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3">
         <v>15</v>
@@ -980,10 +1052,10 @@
         <v>170</v>
       </c>
       <c r="G6" s="3">
-        <v>1450</v>
+        <v>1460</v>
       </c>
       <c r="H6" s="11">
-        <v>0.51</v>
+        <v>0.4</v>
       </c>
       <c r="I6" s="3">
         <v>4</v>
@@ -1001,33 +1073,42 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="N6" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O6" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P6" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q6" s="3">
-        <v>8.6999999999999993</v>
+        <v>60</v>
       </c>
       <c r="R6" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S6" s="3">
-        <v>53</v>
+        <v>38</v>
+      </c>
+      <c r="S6">
+        <v>-0.45</v>
       </c>
       <c r="T6" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>450</v>
+      </c>
+      <c r="U6" s="3">
+        <v>850</v>
+      </c>
+      <c r="V6">
+        <v>11</v>
+      </c>
+      <c r="W6" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3">
         <v>15</v>
@@ -1042,10 +1123,10 @@
         <v>170</v>
       </c>
       <c r="G7" s="3">
-        <v>1640</v>
+        <v>1560</v>
       </c>
       <c r="H7" s="11">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="I7" s="3">
         <v>4</v>
@@ -1057,39 +1138,48 @@
         <v>4</v>
       </c>
       <c r="L7" s="3">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="M7" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N7" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O7" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P7" s="3">
-        <v>880</v>
+        <v>0.26</v>
       </c>
       <c r="Q7" s="3">
-        <v>8.6999999999999993</v>
+        <v>60</v>
       </c>
       <c r="R7" s="3">
-        <v>0.26</v>
-      </c>
-      <c r="S7" s="3">
-        <v>60</v>
+        <v>39</v>
+      </c>
+      <c r="S7">
+        <v>-0.45</v>
       </c>
       <c r="T7" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+        <v>500</v>
+      </c>
+      <c r="U7" s="3">
+        <v>850</v>
+      </c>
+      <c r="V7">
+        <v>11</v>
+      </c>
+      <c r="W7" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3">
         <v>15</v>
@@ -1104,10 +1194,10 @@
         <v>170</v>
       </c>
       <c r="G8" s="3">
-        <v>1550</v>
+        <v>1560</v>
       </c>
       <c r="H8" s="11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I8" s="3">
         <v>4</v>
@@ -1119,47 +1209,347 @@
         <v>4</v>
       </c>
       <c r="L8" s="3">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="M8" s="3">
         <v>1.1499999999999999</v>
       </c>
       <c r="N8" s="3">
-        <v>47</v>
+        <v>880</v>
       </c>
       <c r="O8" s="3">
-        <v>28</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="P8" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>60</v>
+      </c>
+      <c r="R8" s="3">
+        <v>38</v>
+      </c>
+      <c r="S8">
+        <v>-0.45</v>
+      </c>
+      <c r="T8" s="3">
+        <v>500</v>
+      </c>
+      <c r="U8" s="3">
+        <v>850</v>
+      </c>
+      <c r="V8">
+        <v>11</v>
+      </c>
+      <c r="W8" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3">
+        <v>25</v>
+      </c>
+      <c r="F9" s="3">
+        <v>170</v>
+      </c>
+      <c r="G9" s="3">
+        <v>1600</v>
+      </c>
+      <c r="H9" s="11">
+        <f>(0.514*G9 -30.4)/G9</f>
+        <v>0.495</v>
+      </c>
+      <c r="I9" s="3">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K9" s="3">
+        <v>4</v>
+      </c>
+      <c r="L9" s="3">
+        <v>75</v>
+      </c>
+      <c r="M9" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N9" s="3">
         <v>880</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="O9" s="3">
         <v>8.6999999999999993</v>
       </c>
-      <c r="R8" s="3">
+      <c r="P9" s="3">
         <v>0.26</v>
       </c>
-      <c r="S8" s="3">
-        <v>60</v>
-      </c>
-      <c r="T8" s="3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="Q9" s="3">
+        <v>55</v>
+      </c>
+      <c r="R9" s="3">
+        <v>35</v>
+      </c>
+      <c r="S9">
+        <v>-0.45</v>
+      </c>
+      <c r="T9" s="3">
+        <v>460</v>
+      </c>
+      <c r="U9" s="3">
+        <v>850</v>
+      </c>
+      <c r="V9">
+        <v>11</v>
+      </c>
+      <c r="W9" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3">
+        <v>6</v>
+      </c>
+      <c r="E10" s="3">
+        <v>25</v>
+      </c>
+      <c r="F10" s="3">
+        <v>170</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1600</v>
+      </c>
+      <c r="H10" s="11">
+        <f>(G10*0.308 + 273.3)/G10</f>
+        <v>0.47881250000000003</v>
+      </c>
+      <c r="I10" s="3">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K10" s="3">
+        <v>4</v>
+      </c>
+      <c r="L10" s="3">
+        <v>75</v>
+      </c>
+      <c r="M10" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N10" s="3">
+        <v>880</v>
+      </c>
+      <c r="O10" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>55</v>
+      </c>
+      <c r="R10" s="3">
+        <v>35</v>
+      </c>
+      <c r="S10">
+        <v>-0.45</v>
+      </c>
+      <c r="T10" s="3">
+        <v>460</v>
+      </c>
+      <c r="U10" s="3">
+        <v>850</v>
+      </c>
+      <c r="V10">
+        <v>11</v>
+      </c>
+      <c r="W10" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3">
+        <v>25</v>
+      </c>
+      <c r="F11" s="3">
+        <v>170</v>
+      </c>
+      <c r="G11" s="3">
+        <v>1600</v>
+      </c>
+      <c r="H11" s="11">
+        <f>(0.453*G11 + 97.1)/G11</f>
+        <v>0.51368750000000007</v>
+      </c>
+      <c r="I11" s="3">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K11" s="3">
+        <v>4</v>
+      </c>
+      <c r="L11" s="3">
+        <v>75</v>
+      </c>
+      <c r="M11" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N11" s="3">
+        <v>880</v>
+      </c>
+      <c r="O11" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>55</v>
+      </c>
+      <c r="R11" s="3">
+        <v>35</v>
+      </c>
+      <c r="S11">
+        <v>-0.45</v>
+      </c>
+      <c r="T11" s="3">
+        <v>460</v>
+      </c>
+      <c r="U11" s="3">
+        <v>850</v>
+      </c>
+      <c r="V11">
+        <v>11</v>
+      </c>
+      <c r="W11" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3">
+        <v>15</v>
+      </c>
+      <c r="D12" s="3">
+        <v>6</v>
+      </c>
+      <c r="E12" s="3">
+        <v>25</v>
+      </c>
+      <c r="F12" s="3">
+        <v>170</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1600</v>
+      </c>
+      <c r="H12" s="11">
+        <f>(0.41*G12 + 145.4)/G12</f>
+        <v>0.50087499999999996</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="K12" s="3">
+        <v>4</v>
+      </c>
+      <c r="L12" s="3">
+        <v>75</v>
+      </c>
+      <c r="M12" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N12" s="3">
+        <v>880</v>
+      </c>
+      <c r="O12" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>55</v>
+      </c>
+      <c r="R12" s="3">
+        <v>35</v>
+      </c>
+      <c r="S12">
+        <v>-0.45</v>
+      </c>
+      <c r="T12" s="3">
+        <v>460</v>
+      </c>
+      <c r="U12" s="3">
+        <v>850</v>
+      </c>
+      <c r="V12">
+        <v>11</v>
+      </c>
+      <c r="W12" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="F15"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>